<commit_message>
lease_realty load data partial 2
</commit_message>
<xml_diff>
--- a/_files/lease_realties_pending.xlsx
+++ b/_files/lease_realties_pending.xlsx
@@ -8,19 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\leon\projects\adin_2022\_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E0E13E-B7A3-421C-B338-FEA7FD6130D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0147D86D-D343-4483-8088-D0B73A9DF099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1410" windowWidth="11550" windowHeight="10290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lease_realties_pending" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="105">
   <si>
     <t>realty</t>
   </si>
@@ -342,7 +354,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -480,7 +492,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -658,12 +670,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -827,11 +833,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1191,10 +1196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N103"/>
+  <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:C29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1202,10 +1207,10 @@
     <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1226,13 +1231,13 @@
       <c r="E1" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1249,11 +1254,11 @@
       <c r="E2" s="1">
         <v>44562</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="H2" s="6">
+      <c r="F2" s="4"/>
+      <c r="H2" s="5">
         <v>19128434</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>6108014</v>
       </c>
     </row>
@@ -1270,14 +1275,14 @@
       <c r="E3" s="1">
         <v>44562</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="3">
+      <c r="F3" s="4"/>
+      <c r="G3" s="2">
         <v>1100000</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>19128434</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>1143861826</v>
       </c>
     </row>
@@ -1294,66 +1299,66 @@
       <c r="E4" s="1">
         <v>44562</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="3">
+      <c r="F4" s="4"/>
+      <c r="G4" s="2">
         <v>940000</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>19128434</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>1193172681</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>43983</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>43983</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>44681</v>
       </c>
-      <c r="E5" s="5">
-        <v>44562</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="3">
+      <c r="E5" s="4">
+        <v>44562</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="2">
         <v>790000</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>19128434</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>1077470443</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>44682</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>44682</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5">
+      <c r="D6" s="3"/>
+      <c r="E6" s="4">
         <v>44682</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="3">
+      <c r="F6" s="4"/>
+      <c r="G6" s="2">
         <v>790000</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>19128434</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>352403</v>
       </c>
     </row>
@@ -1370,14 +1375,14 @@
       <c r="E7" s="1">
         <v>44562</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="3">
+      <c r="F7" s="4"/>
+      <c r="G7" s="2">
         <v>840000</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>19128434</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>1032370914</v>
       </c>
     </row>
@@ -1394,14 +1399,14 @@
       <c r="E8" s="1">
         <v>44562</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="3">
+      <c r="F8" s="4"/>
+      <c r="G8" s="2">
         <v>850000</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>19128434</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>66725374</v>
       </c>
     </row>
@@ -1428,14 +1433,14 @@
       <c r="E11" s="1">
         <v>44562</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="3">
+      <c r="F11" s="4"/>
+      <c r="G11" s="2">
         <v>480000</v>
       </c>
-      <c r="H11" s="6">
-        <v>6108014</v>
-      </c>
-      <c r="I11" s="6">
+      <c r="H11" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I11" s="5">
         <v>1130668637</v>
       </c>
     </row>
@@ -1452,14 +1457,14 @@
       <c r="E12" s="1">
         <v>44562</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="3">
+      <c r="F12" s="4"/>
+      <c r="G12" s="2">
         <v>450000</v>
       </c>
-      <c r="H12" s="6">
-        <v>6108014</v>
-      </c>
-      <c r="I12" s="6">
+      <c r="H12" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I12" s="5">
         <v>31836102</v>
       </c>
     </row>
@@ -1476,14 +1481,14 @@
       <c r="E13" s="1">
         <v>44562</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="3">
+      <c r="F13" s="4"/>
+      <c r="G13" s="2">
         <v>530000</v>
       </c>
-      <c r="H13" s="6">
-        <v>6108014</v>
-      </c>
-      <c r="I13" s="6">
+      <c r="H13" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I13" s="5">
         <v>1144207981</v>
       </c>
     </row>
@@ -1503,14 +1508,14 @@
       <c r="E14" s="1">
         <v>44562</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="3">
+      <c r="F14" s="4"/>
+      <c r="G14" s="2">
         <v>700000</v>
       </c>
-      <c r="H14" s="6">
-        <v>6108014</v>
-      </c>
-      <c r="I14" s="6">
+      <c r="H14" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I14" s="5">
         <v>31214798</v>
       </c>
     </row>
@@ -1528,14 +1533,14 @@
       <c r="E15" s="1">
         <v>44737</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="3">
+      <c r="F15" s="4"/>
+      <c r="G15" s="2">
         <v>650000</v>
       </c>
-      <c r="H15" s="6">
-        <v>6108014</v>
-      </c>
-      <c r="I15" s="6">
+      <c r="H15" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I15" s="5">
         <v>16792693</v>
       </c>
     </row>
@@ -1552,11 +1557,11 @@
       <c r="E16" s="1">
         <v>44562</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="H16" s="6">
-        <v>6108014</v>
-      </c>
-      <c r="I16" s="6">
+      <c r="F16" s="4"/>
+      <c r="H16" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I16" s="5">
         <v>19245383</v>
       </c>
     </row>
@@ -1573,14 +1578,14 @@
       <c r="E17" s="1">
         <v>44562</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="3">
+      <c r="F17" s="4"/>
+      <c r="G17" s="2">
         <v>530000</v>
       </c>
-      <c r="H17" s="6">
-        <v>6108014</v>
-      </c>
-      <c r="I17" s="6">
+      <c r="H17" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I17" s="5">
         <v>19160350</v>
       </c>
     </row>
@@ -1597,14 +1602,14 @@
       <c r="E18" s="1">
         <v>44562</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="3">
+      <c r="F18" s="4"/>
+      <c r="G18" s="2">
         <v>830000</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <v>19128434</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <v>31641849</v>
       </c>
     </row>
@@ -1621,14 +1626,14 @@
       <c r="E19" s="1">
         <v>44562</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="3">
+      <c r="F19" s="4"/>
+      <c r="G19" s="2">
         <v>700000</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <v>19128434</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <v>1144101694</v>
       </c>
     </row>
@@ -1648,7 +1653,7 @@
       <c r="E20" s="1">
         <v>44562</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -1664,14 +1669,14 @@
       <c r="E21" s="1">
         <v>44652</v>
       </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="3">
+      <c r="F21" s="4"/>
+      <c r="G21" s="2">
         <v>700000</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <v>19128434</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="5">
         <v>1118290288</v>
       </c>
     </row>
@@ -1688,14 +1693,14 @@
       <c r="E22" s="1">
         <v>44562</v>
       </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="3">
+      <c r="F22" s="4"/>
+      <c r="G22" s="2">
         <v>650000</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <v>19128434</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="5">
         <v>1116446148</v>
       </c>
     </row>
@@ -1712,14 +1717,14 @@
       <c r="E23" s="1">
         <v>44562</v>
       </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="3">
+      <c r="F23" s="4"/>
+      <c r="G23" s="2">
         <v>750000</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="5">
         <v>19128434</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="5">
         <v>1144077780</v>
       </c>
     </row>
@@ -1732,10 +1737,10 @@
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>38047</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>38047</v>
       </c>
       <c r="D25" s="1">
@@ -1744,14 +1749,14 @@
       <c r="E25" s="1">
         <v>44562</v>
       </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="3">
+      <c r="F25" s="4"/>
+      <c r="G25" s="2">
         <v>240000</v>
       </c>
-      <c r="H25" s="6">
-        <v>6108014</v>
-      </c>
-      <c r="I25" s="6">
+      <c r="H25" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I25" s="5">
         <v>31205367</v>
       </c>
     </row>
@@ -1768,14 +1773,14 @@
       <c r="E26" s="1">
         <v>44562</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="3">
+      <c r="F26" s="4"/>
+      <c r="G26" s="2">
         <v>390000</v>
       </c>
-      <c r="H26" s="6">
-        <v>6108014</v>
-      </c>
-      <c r="I26" s="6">
+      <c r="H26" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I26" s="5">
         <v>16592209</v>
       </c>
     </row>
@@ -1792,14 +1797,14 @@
       <c r="E27" s="1">
         <v>44551</v>
       </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="3">
+      <c r="F27" s="4"/>
+      <c r="G27" s="2">
         <v>260000</v>
       </c>
-      <c r="H27" s="6">
-        <v>6108014</v>
-      </c>
-      <c r="I27" s="6">
+      <c r="H27" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I27" s="5">
         <v>6085201</v>
       </c>
     </row>
@@ -1813,31 +1818,43 @@
       <c r="C28" s="1">
         <v>42814</v>
       </c>
+      <c r="D28" s="1">
+        <v>44639</v>
+      </c>
       <c r="E28" s="1">
         <v>44550</v>
       </c>
-      <c r="F28" s="5"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="2">
+        <v>400000</v>
+      </c>
+      <c r="H28" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I28" s="5">
+        <v>1130668637</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <v>42802</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>42802</v>
       </c>
       <c r="E29" s="1">
         <v>44569</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="2">
         <v>390000</v>
       </c>
-      <c r="H29" s="6">
-        <v>6108014</v>
-      </c>
-      <c r="I29" s="6">
+      <c r="H29" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I29" s="5">
         <v>14956720</v>
       </c>
     </row>
@@ -1854,7 +1871,16 @@
       <c r="E30" s="1">
         <v>44562</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="2">
+        <v>370000</v>
+      </c>
+      <c r="H30" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I30" s="5">
+        <v>17097961</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
@@ -1869,19 +1895,28 @@
       <c r="E31" s="1">
         <v>44562</v>
       </c>
-      <c r="F31" s="5"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="2">
+        <v>430000</v>
+      </c>
+      <c r="H31" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I31" s="5">
+        <v>39774268</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1894,14 +1929,23 @@
       <c r="E34" s="1">
         <v>44501</v>
       </c>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F34" s="4"/>
+      <c r="G34" s="2">
+        <v>430000</v>
+      </c>
+      <c r="H34" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I34" s="5">
+        <v>31485759</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1914,34 +1958,70 @@
       <c r="E36" s="1">
         <v>44562</v>
       </c>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F36" s="4"/>
+      <c r="G36" s="2">
+        <v>220000</v>
+      </c>
+      <c r="H36" s="5">
+        <v>19128434</v>
+      </c>
+      <c r="I36" s="5">
+        <v>33922</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="4">
         <v>43266</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="4">
         <v>43266</v>
       </c>
       <c r="E38" s="1">
         <v>44576</v>
       </c>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F38" s="4"/>
+      <c r="G38" s="2">
+        <v>310000</v>
+      </c>
+      <c r="H38" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I38" s="5">
+        <v>29054785</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B39" s="1">
+        <v>44713</v>
+      </c>
+      <c r="C39" s="1">
+        <v>44713</v>
+      </c>
+      <c r="E39" s="1">
+        <v>44713</v>
+      </c>
+      <c r="G39" s="2">
+        <v>570000</v>
+      </c>
+      <c r="H39" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I39" s="5">
+        <v>19845080</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1951,12 +2031,24 @@
       <c r="C40" s="1">
         <v>44409</v>
       </c>
+      <c r="D40" s="1">
+        <v>44773</v>
+      </c>
       <c r="E40" s="1">
         <v>44562</v>
       </c>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F40" s="4"/>
+      <c r="G40" s="2">
+        <v>830000</v>
+      </c>
+      <c r="H40" s="5">
+        <v>19128434</v>
+      </c>
+      <c r="I40" s="5">
+        <v>29434066</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1966,12 +2058,22 @@
       <c r="C41" s="1">
         <v>44409</v>
       </c>
+      <c r="D41" s="1"/>
       <c r="E41" s="1">
         <v>44531</v>
       </c>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F41" s="4"/>
+      <c r="G41" s="2">
+        <v>700000</v>
+      </c>
+      <c r="H41" s="5">
+        <v>19128434</v>
+      </c>
+      <c r="I41" s="5">
+        <v>1086017</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1979,646 +2081,870 @@
         <v>44621</v>
       </c>
       <c r="C42" s="1">
-        <v>44621</v>
+        <v>44599</v>
       </c>
       <c r="E42" s="1">
         <v>44599</v>
       </c>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F42" s="4"/>
+      <c r="G42" s="2">
+        <v>700000</v>
+      </c>
+      <c r="H42" s="5">
+        <v>19128434</v>
+      </c>
+      <c r="I42" s="5">
+        <v>1113686599</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="4">
         <v>44652</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C44" s="4">
         <v>44652</v>
       </c>
-      <c r="E43" s="2">
+      <c r="D44" s="3"/>
+      <c r="E44" s="4">
         <v>44652</v>
       </c>
-      <c r="F43" s="5"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="F44" s="4"/>
+      <c r="G44" s="2">
+        <v>700000</v>
+      </c>
+      <c r="H44" s="5">
+        <v>19128434</v>
+      </c>
+      <c r="I44" s="5">
+        <v>31197760</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B45" s="1">
         <v>44228</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C45" s="1">
         <v>44228</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E45" s="1">
         <v>44197</v>
       </c>
-      <c r="F44" s="5"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="F45" s="4"/>
+      <c r="G45" s="2">
+        <v>750000</v>
+      </c>
+      <c r="H45" s="5">
+        <v>19128434</v>
+      </c>
+      <c r="I45" s="5">
+        <v>1115073326</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B46" s="1">
         <v>43252</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C46" s="1">
         <v>43252</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E46" s="1">
         <v>44501</v>
       </c>
-      <c r="F45" s="5"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="F46" s="4"/>
+      <c r="G46" s="2">
+        <v>420000</v>
+      </c>
+      <c r="H46" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I46" s="5">
+        <v>16701786</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="1">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="1">
+        <v>44743</v>
+      </c>
+      <c r="C49" s="1">
+        <v>44743</v>
+      </c>
+      <c r="E49" s="1">
+        <v>44743</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="2">
+        <v>390000</v>
+      </c>
+      <c r="H49" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I49" s="5">
+        <v>1114728401</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="1">
         <v>44621</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C50" s="1">
         <v>44621</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E50" s="1">
         <v>44621</v>
       </c>
-      <c r="F47" s="5"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" s="1">
+      <c r="F50" s="4"/>
+      <c r="G50" s="2">
+        <v>390000</v>
+      </c>
+      <c r="H50" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I50" s="5">
+        <v>61437235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="1">
+        <v>44743</v>
+      </c>
+      <c r="C52" s="1">
+        <v>44743</v>
+      </c>
+      <c r="E52" s="1">
+        <v>44743</v>
+      </c>
+      <c r="G52" s="2">
+        <v>390000</v>
+      </c>
+      <c r="H52" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I52" s="5">
+        <v>29185053</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" s="1">
+        <v>44501</v>
+      </c>
+      <c r="C53" s="1">
+        <v>44490</v>
+      </c>
+      <c r="E53" s="1">
+        <v>44562</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="2">
+        <v>390000</v>
+      </c>
+      <c r="H53" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I53" s="5">
+        <v>1130628991</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="1">
+        <v>42887</v>
+      </c>
+      <c r="C54" s="1">
+        <v>42887</v>
+      </c>
+      <c r="E54" s="1">
+        <v>44562</v>
+      </c>
+      <c r="F54" s="4"/>
+      <c r="G54" s="2">
+        <v>420000</v>
+      </c>
+      <c r="H54" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I54" s="5">
+        <v>1130668637</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="1">
+        <v>43617</v>
+      </c>
+      <c r="C55" s="1">
+        <v>43617</v>
+      </c>
+      <c r="E55" s="1">
+        <v>44562</v>
+      </c>
+      <c r="F55" s="4"/>
+      <c r="G55" s="2">
+        <v>430000</v>
+      </c>
+      <c r="H55" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I55" s="5">
+        <v>66818737</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="1">
+        <v>43678</v>
+      </c>
+      <c r="C56" s="1">
+        <v>43678</v>
+      </c>
+      <c r="D56" s="1">
+        <v>44742</v>
+      </c>
+      <c r="E56" s="1">
+        <v>44562</v>
+      </c>
+      <c r="G56" s="2">
+        <v>295000</v>
+      </c>
+      <c r="H56" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I56" s="5">
+        <v>1114728401</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58" s="1">
+        <v>44713</v>
+      </c>
+      <c r="C58" s="1">
+        <v>44715</v>
+      </c>
+      <c r="E58" s="1">
+        <v>44715</v>
+      </c>
+      <c r="G58" s="2">
+        <v>390000</v>
+      </c>
+      <c r="H58" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I58" s="5">
+        <v>1125230924</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59" s="1">
+        <v>44409</v>
+      </c>
+      <c r="C59" s="1">
+        <v>44409</v>
+      </c>
+      <c r="E59" s="1">
+        <v>44562</v>
+      </c>
+      <c r="G59" s="2">
+        <v>290000</v>
+      </c>
+      <c r="H59" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I59" s="5">
+        <v>80817426</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60" s="1">
+        <v>44409</v>
+      </c>
+      <c r="C60" s="1">
+        <v>44409</v>
+      </c>
+      <c r="E60" s="1">
+        <v>44562</v>
+      </c>
+      <c r="G60" s="2">
+        <v>470000</v>
+      </c>
+      <c r="H60" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I60" s="5">
+        <v>79052475</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62" s="1">
+        <v>35290</v>
+      </c>
+      <c r="C62" s="1">
+        <v>35290</v>
+      </c>
+      <c r="E62" s="1">
+        <v>44562</v>
+      </c>
+      <c r="G62" s="2">
+        <v>150000</v>
+      </c>
+      <c r="H62" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I62" s="5">
+        <v>31233821</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" s="1">
+        <v>44197</v>
+      </c>
+      <c r="C63" s="1">
+        <v>44197</v>
+      </c>
+      <c r="E63" s="1">
+        <v>44562</v>
+      </c>
+      <c r="G63" s="2">
+        <v>470000</v>
+      </c>
+      <c r="H63" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I63" s="5">
+        <v>94041536</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" s="1">
+        <v>43556</v>
+      </c>
+      <c r="C64" s="1">
+        <v>43556</v>
+      </c>
+      <c r="E64" s="1">
+        <v>44562</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="2">
+        <v>700000</v>
+      </c>
+      <c r="H64" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="I64" s="5">
+        <v>70903810</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" s="1">
+        <v>36192</v>
+      </c>
+      <c r="C65" s="1">
+        <v>36192</v>
+      </c>
+      <c r="E65" s="1">
+        <v>44562</v>
+      </c>
+      <c r="F65" s="4"/>
+      <c r="G65" s="2">
+        <v>1120000</v>
+      </c>
+      <c r="H65" s="5">
+        <v>19245383</v>
+      </c>
+      <c r="I65" s="5">
+        <v>70903810</v>
+      </c>
+      <c r="K65" s="1"/>
+      <c r="M65" s="1"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" s="1">
+        <v>44470</v>
+      </c>
+      <c r="C66" s="1">
+        <v>44470</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67" s="1">
         <v>44621</v>
       </c>
-      <c r="C48" s="1">
-        <v>44621</v>
-      </c>
-      <c r="E48" s="1">
-        <v>44621</v>
-      </c>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" s="1">
-        <v>44501</v>
-      </c>
-      <c r="C50" s="1">
-        <v>44501</v>
-      </c>
-      <c r="E50" s="1">
-        <v>44562</v>
-      </c>
-      <c r="F50" s="5"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="1">
-        <v>39234</v>
-      </c>
-      <c r="C51" s="1">
-        <v>39234</v>
-      </c>
-      <c r="E51" s="1">
-        <v>44562</v>
-      </c>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" s="1">
-        <v>43617</v>
-      </c>
-      <c r="C52" s="1">
-        <v>43617</v>
-      </c>
-      <c r="E52" s="1">
-        <v>44562</v>
-      </c>
-      <c r="F52" s="5"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="1">
+      <c r="C67" s="1">
+        <v>44631</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>64</v>
+      </c>
+      <c r="B68" s="1">
+        <v>44228</v>
+      </c>
+      <c r="C68" s="1">
+        <v>44228</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70" s="1">
+        <v>42856</v>
+      </c>
+      <c r="C70" s="1">
+        <v>42856</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>67</v>
+      </c>
+      <c r="B71" s="1">
+        <v>44136</v>
+      </c>
+      <c r="C71" s="1">
+        <v>44136</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72" s="1">
+        <v>41379</v>
+      </c>
+      <c r="C72" s="1">
+        <v>41379</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73" s="1">
+        <v>43009</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" s="1">
         <v>43556</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C74" s="1">
         <v>43556</v>
       </c>
-      <c r="E61" s="1">
-        <v>44562</v>
-      </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="3">
-        <v>700000</v>
-      </c>
-      <c r="H61" s="6">
-        <v>6108014</v>
-      </c>
-      <c r="I61" s="6">
-        <v>70903810</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" s="1">
-        <v>36192</v>
-      </c>
-      <c r="C62" s="1">
-        <v>36192</v>
-      </c>
-      <c r="E62" s="1">
-        <v>44562</v>
-      </c>
-      <c r="F62" s="5"/>
-      <c r="G62" s="3">
-        <v>1120000</v>
-      </c>
-      <c r="H62" s="6">
-        <v>19245383</v>
-      </c>
-      <c r="I62" s="6">
-        <v>70903810</v>
-      </c>
-      <c r="K62" s="1">
-        <v>44228</v>
-      </c>
-      <c r="L62">
-        <v>2600000</v>
-      </c>
-      <c r="M62" s="1">
-        <v>44593</v>
-      </c>
-      <c r="N62">
-        <v>2720000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63" s="1">
-        <v>44470</v>
-      </c>
-      <c r="C63" s="1">
-        <v>44470</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" s="1">
-        <v>44621</v>
-      </c>
-      <c r="C64" s="1">
-        <v>44631</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" s="1">
-        <v>44228</v>
-      </c>
-      <c r="C65" s="1">
-        <v>44228</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" s="1">
-        <v>42856</v>
-      </c>
-      <c r="C67" s="1">
-        <v>42856</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>67</v>
-      </c>
-      <c r="B68" s="1">
-        <v>44136</v>
-      </c>
-      <c r="C68" s="1">
-        <v>44136</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>68</v>
-      </c>
-      <c r="B69" s="1">
-        <v>41379</v>
-      </c>
-      <c r="C69" s="1">
-        <v>41379</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>69</v>
-      </c>
-      <c r="B70" s="1">
-        <v>43009</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>70</v>
-      </c>
-      <c r="B71" s="1">
-        <v>43556</v>
-      </c>
-      <c r="C71" s="1">
-        <v>43556</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B75" s="1">
         <v>41883</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C75" s="1">
         <v>41883</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B76" s="1">
         <v>43770</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C76" s="1">
         <v>43770</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B77" s="1">
         <v>42415</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>73</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B78" s="1">
         <v>43221</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C78" s="1">
         <v>43221</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>74</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B79" s="1">
         <v>38200</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C79" s="1">
         <v>38200</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>75</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B80" s="1">
         <v>39814</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C80" s="1">
         <v>39814</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>76</v>
-      </c>
-      <c r="B78" s="1">
-        <v>41611</v>
-      </c>
-      <c r="C78" s="1">
-        <v>41611</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>77</v>
-      </c>
-      <c r="B79" s="1">
-        <v>42415</v>
-      </c>
-      <c r="C79" s="1">
-        <v>42415</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>78</v>
-      </c>
-      <c r="B80" s="1">
-        <v>43435</v>
-      </c>
-      <c r="C80" s="1">
-        <v>43435</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B81" s="1">
-        <v>41250</v>
+        <v>41611</v>
       </c>
       <c r="C81" s="1">
-        <v>41244</v>
+        <v>41611</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B82" s="1">
-        <v>41426</v>
+        <v>42415</v>
       </c>
       <c r="C82" s="1">
-        <v>41426</v>
+        <v>42415</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B83" s="1">
-        <v>40940</v>
+        <v>43435</v>
+      </c>
+      <c r="C83" s="1">
+        <v>43435</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B84" s="1">
-        <v>42931</v>
+        <v>41250</v>
+      </c>
+      <c r="C84" s="1">
+        <v>41244</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B85" s="1">
-        <v>44470</v>
+        <v>41426</v>
       </c>
       <c r="C85" s="1">
-        <v>44470</v>
+        <v>41426</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B86" s="1">
-        <v>42887</v>
-      </c>
-      <c r="C86" s="1">
-        <v>42887</v>
+        <v>40940</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B87" s="1">
-        <v>37135</v>
-      </c>
-      <c r="C87" s="1">
-        <v>37135</v>
+        <v>42931</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="B88" s="1">
+        <v>44470</v>
+      </c>
+      <c r="C88" s="1">
+        <v>44470</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B89" s="1">
-        <v>44044</v>
+        <v>42887</v>
       </c>
       <c r="C89" s="1">
-        <v>44044</v>
+        <v>42887</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B90" s="1">
-        <v>44440</v>
+        <v>37135</v>
       </c>
       <c r="C90" s="1">
-        <v>44440</v>
+        <v>37135</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>89</v>
-      </c>
-      <c r="B91" s="1">
-        <v>38847</v>
-      </c>
-      <c r="C91" s="1">
-        <v>38847</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B92" s="1">
-        <v>41518</v>
+        <v>44044</v>
       </c>
       <c r="C92" s="1">
-        <v>41518</v>
+        <v>44044</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B93" s="1">
-        <v>25569</v>
+        <v>44440</v>
+      </c>
+      <c r="C93" s="1">
+        <v>44440</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B94" s="1">
-        <v>43221</v>
+        <v>38847</v>
       </c>
       <c r="C94" s="1">
-        <v>43221</v>
+        <v>38847</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="B95" s="1">
+        <v>41518</v>
+      </c>
+      <c r="C95" s="1">
+        <v>41518</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B96" s="1">
-        <v>42826</v>
-      </c>
-      <c r="C96" s="1">
-        <v>42826</v>
+        <v>25569</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B97" s="1">
-        <v>43647</v>
+        <v>43221</v>
       </c>
       <c r="C97" s="1">
-        <v>43647</v>
+        <v>43221</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>95</v>
-      </c>
-      <c r="B98" s="1">
-        <v>41426</v>
-      </c>
-      <c r="C98" s="1">
-        <v>41426</v>
+        <v>92</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B99" s="1">
-        <v>44105</v>
+        <v>42826</v>
       </c>
       <c r="C99" s="1">
-        <v>44105</v>
+        <v>42826</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B100" s="1">
-        <v>43770</v>
+        <v>43647</v>
       </c>
       <c r="C100" s="1">
-        <v>43770</v>
+        <v>43647</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>98</v>
+        <v>95</v>
+      </c>
+      <c r="B101" s="1">
+        <v>41426</v>
+      </c>
+      <c r="C101" s="1">
+        <v>41426</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B102" s="1">
-        <v>44531</v>
+        <v>44105</v>
       </c>
       <c r="C102" s="1">
-        <v>44545</v>
+        <v>44105</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
+        <v>97</v>
+      </c>
+      <c r="B103" s="1">
+        <v>43770</v>
+      </c>
+      <c r="C103" s="1">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>99</v>
+      </c>
+      <c r="B105" s="1">
+        <v>44531</v>
+      </c>
+      <c r="C105" s="1">
+        <v>44545</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
debug create accon partial
</commit_message>
<xml_diff>
--- a/_files/lease_realties_pending.xlsx
+++ b/_files/lease_realties_pending.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\leon\projects\adin_2022\_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0147D86D-D343-4483-8088-D0B73A9DF099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC53DB7A-7FC5-47E3-903A-319F77CE2548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1410" windowWidth="11550" windowHeight="10290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32410" yWindow="7340" windowWidth="11550" windowHeight="10290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lease_realties_pending" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="107">
   <si>
     <t>realty</t>
   </si>
@@ -347,6 +347,12 @@
   </si>
   <si>
     <t>valor</t>
+  </si>
+  <si>
+    <t>CONCAT(A2,"^",YEAR(B2),"-",IF(MONTH(B2)&lt;10,CONCAT("0",MONTH(B2)),MONTH(B2)),"-",IF(DAY(B2)&lt;10,CONCAT("0",DAY(B2)),DAY(B2)))</t>
+  </si>
+  <si>
+    <t>Destrate</t>
   </si>
 </sst>
 </file>
@@ -1196,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M106"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1207,12 +1213,10 @@
     <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -1231,14 +1235,17 @@
       <c r="E1" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>104</v>
       </c>
+      <c r="G1" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="H1" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="I1" s="5" t="s">
         <v>102</v>
+      </c>
+      <c r="I1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1254,12 +1261,15 @@
       <c r="E2" s="1">
         <v>44562</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="G2" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H2" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I2" s="5">
-        <v>6108014</v>
+        <v>6108014</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2:I8" si="0">_xlfn.CONCAT(A2,"^",YEAR(B2),"-",IF(MONTH(B2)&lt;10,_xlfn.CONCAT("0",MONTH(B2)),MONTH(B2)),"-",IF(DAY(B2)&lt;10,_xlfn.CONCAT("0",DAY(B2)),DAY(B2)))</f>
+        <v>A6N-13N-62-O1^2015-01-01</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1275,15 +1285,18 @@
       <c r="E3" s="1">
         <v>44562</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2">
+      <c r="F3" s="2">
         <v>1100000</v>
       </c>
+      <c r="G3" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H3" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I3" s="5">
         <v>1143861826</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="0"/>
+        <v>A6N-13N-62-S101^2021-04-01</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1299,15 +1312,18 @@
       <c r="E4" s="1">
         <v>44562</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2">
+      <c r="F4" s="2">
         <v>940000</v>
       </c>
+      <c r="G4" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H4" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I4" s="5">
         <v>1193172681</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>A6N-13N-62-S102^2021-10-01</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1326,15 +1342,18 @@
       <c r="E5" s="4">
         <v>44562</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2">
+      <c r="F5" s="2">
         <v>790000</v>
       </c>
+      <c r="G5" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H5" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I5" s="5">
         <v>1077470443</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>A6N-13N-62-S103^2020-06-01</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1351,15 +1370,18 @@
       <c r="E6" s="4">
         <v>44682</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="2">
+      <c r="F6" s="2">
         <v>790000</v>
       </c>
+      <c r="G6" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H6" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I6" s="5">
         <v>352403</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>A6N-13N-62-S103^2022-05-01</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1375,15 +1397,18 @@
       <c r="E7" s="1">
         <v>44562</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="2">
+      <c r="F7" s="2">
         <v>840000</v>
       </c>
+      <c r="G7" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H7" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I7" s="5">
         <v>1032370914</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>A6N-13N-62-S104^2021-08-01</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1399,15 +1424,18 @@
       <c r="E8" s="1">
         <v>44562</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="2">
+      <c r="F8" s="2">
         <v>850000</v>
       </c>
+      <c r="G8" s="6">
+        <v>19128434</v>
+      </c>
       <c r="H8" s="6">
-        <v>19128434</v>
-      </c>
-      <c r="I8" s="6">
         <v>66725374</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>A6N-13N-62-S105^2021-09-01</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1433,15 +1461,18 @@
       <c r="E11" s="1">
         <v>44562</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="2">
+      <c r="F11" s="2">
         <v>480000</v>
       </c>
+      <c r="G11" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H11" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I11" s="5">
         <v>1130668637</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" ref="I11:I23" si="1">_xlfn.CONCAT(A11,"^",YEAR(B11),"-",IF(MONTH(B11)&lt;10,_xlfn.CONCAT("0",MONTH(B11)),MONTH(B11)),"-",IF(DAY(B11)&lt;10,_xlfn.CONCAT("0",DAY(B11)),DAY(B11)))</f>
+        <v>A6N-13N-62-S108^2016-12-01</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1457,15 +1488,18 @@
       <c r="E12" s="1">
         <v>44562</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="2">
+      <c r="F12" s="2">
         <v>450000</v>
       </c>
+      <c r="G12" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H12" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I12" s="5">
         <v>31836102</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v>A6N-13N-62-S109^2021-07-01</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1481,15 +1515,18 @@
       <c r="E13" s="1">
         <v>44562</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="2">
+      <c r="F13" s="2">
         <v>530000</v>
       </c>
+      <c r="G13" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H13" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I13" s="5">
         <v>1144207981</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="1"/>
+        <v>A6N-13N-62-S110^2021-09-01</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1508,15 +1545,18 @@
       <c r="E14" s="1">
         <v>44562</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="2">
+      <c r="F14" s="2">
         <v>700000</v>
       </c>
+      <c r="G14" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H14" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I14" s="5">
         <v>31214798</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v>A6N-13N-62-S111^2021-04-01</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1533,15 +1573,18 @@
       <c r="E15" s="1">
         <v>44737</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="2">
+      <c r="F15" s="2">
         <v>650000</v>
       </c>
+      <c r="G15" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H15" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I15" s="5">
         <v>16792693</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v>A6N-13N-62-S111^2022-07-01</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1557,12 +1600,15 @@
       <c r="E16" s="1">
         <v>44562</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="G16" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H16" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I16" s="5">
         <v>19245383</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v>A6N-13N-62-S112^2015-04-01</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1578,15 +1624,18 @@
       <c r="E17" s="1">
         <v>44562</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="2">
+      <c r="F17" s="2">
         <v>530000</v>
       </c>
+      <c r="G17" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H17" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I17" s="5">
         <v>19160350</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="1"/>
+        <v>A6N-13N-62-S114^2021-09-01</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1602,15 +1651,18 @@
       <c r="E18" s="1">
         <v>44562</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="2">
+      <c r="F18" s="2">
         <v>830000</v>
       </c>
+      <c r="G18" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H18" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I18" s="5">
         <v>31641849</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="1"/>
+        <v>A6N-13N-62-S201^2021-10-01</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1626,15 +1678,18 @@
       <c r="E19" s="1">
         <v>44562</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="2">
+      <c r="F19" s="2">
         <v>700000</v>
       </c>
+      <c r="G19" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H19" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I19" s="5">
         <v>1144101694</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="1"/>
+        <v>A6N-13N-62-S202^2021-10-01</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1653,7 +1708,10 @@
       <c r="E20" s="1">
         <v>44562</v>
       </c>
-      <c r="F20" s="4"/>
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v>A6N-13N-62-S203^2020-10-01</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -1669,15 +1727,18 @@
       <c r="E21" s="1">
         <v>44652</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="2">
+      <c r="F21" s="2">
         <v>700000</v>
       </c>
+      <c r="G21" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H21" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I21" s="5">
         <v>1118290288</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
+        <v>A6N-13N-62-S203^2022-04-01</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1693,15 +1754,18 @@
       <c r="E22" s="1">
         <v>44562</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="2">
+      <c r="F22" s="2">
         <v>650000</v>
       </c>
+      <c r="G22" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H22" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I22" s="5">
         <v>1116446148</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v>A6N-13N-62-S204^2021-09-01</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1717,15 +1781,18 @@
       <c r="E23" s="1">
         <v>44562</v>
       </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="2">
+      <c r="F23" s="2">
         <v>750000</v>
       </c>
+      <c r="G23" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H23" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I23" s="5">
         <v>1144077780</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="1"/>
+        <v>A6N-13N-62-S205^2020-08-01</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1749,15 +1816,18 @@
       <c r="E25" s="1">
         <v>44562</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="2">
+      <c r="F25" s="2">
         <v>240000</v>
       </c>
+      <c r="G25" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H25" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I25" s="5">
         <v>31205367</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" ref="I25:I31" si="2">_xlfn.CONCAT(A25,"^",YEAR(B25),"-",IF(MONTH(B25)&lt;10,_xlfn.CONCAT("0",MONTH(B25)),MONTH(B25)),"-",IF(DAY(B25)&lt;10,_xlfn.CONCAT("0",DAY(B25)),DAY(B25)))</f>
+        <v>A6N-13N-62-S207^2004-03-01</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1773,15 +1843,18 @@
       <c r="E26" s="1">
         <v>44562</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="2">
+      <c r="F26" s="2">
         <v>390000</v>
       </c>
+      <c r="G26" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H26" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I26" s="5">
         <v>16592209</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="2"/>
+        <v>A6N-13N-62-S208^2021-10-01</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -1797,15 +1870,18 @@
       <c r="E27" s="1">
         <v>44551</v>
       </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="2">
+      <c r="F27" s="2">
         <v>260000</v>
       </c>
+      <c r="G27" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H27" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I27" s="5">
         <v>6085201</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="2"/>
+        <v>A6N-13N-62-S209^2006-03-21</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -1824,15 +1900,18 @@
       <c r="E28" s="1">
         <v>44550</v>
       </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="2">
+      <c r="F28" s="2">
         <v>400000</v>
       </c>
+      <c r="G28" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H28" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I28" s="5">
         <v>1130668637</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="2"/>
+        <v>A6N-13N-62-S210^2017-03-20</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -1848,14 +1927,18 @@
       <c r="E29" s="1">
         <v>44569</v>
       </c>
-      <c r="G29" s="2">
+      <c r="F29" s="2">
         <v>390000</v>
       </c>
+      <c r="G29" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H29" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I29" s="5">
         <v>14956720</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="2"/>
+        <v>A6N-13N-62-S211^2017-03-08</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -1871,15 +1954,18 @@
       <c r="E30" s="1">
         <v>44562</v>
       </c>
-      <c r="F30" s="4"/>
-      <c r="G30" s="2">
+      <c r="F30" s="2">
         <v>370000</v>
       </c>
+      <c r="G30" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H30" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I30" s="5">
         <v>17097961</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="2"/>
+        <v>A6N-13N-62-S212^2011-09-01</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -1895,15 +1981,18 @@
       <c r="E31" s="1">
         <v>44562</v>
       </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="2">
+      <c r="F31" s="2">
         <v>430000</v>
       </c>
+      <c r="G31" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H31" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I31" s="5">
         <v>39774268</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="2"/>
+        <v>A6N-13N-62-S214^2018-10-01</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -1929,15 +2018,18 @@
       <c r="E34" s="1">
         <v>44501</v>
       </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="2">
+      <c r="F34" s="2">
         <v>430000</v>
       </c>
+      <c r="G34" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H34" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I34" s="5">
         <v>31485759</v>
+      </c>
+      <c r="I34" t="str">
+        <f>_xlfn.CONCAT(A34,"^",YEAR(B34),"-",IF(MONTH(B34)&lt;10,_xlfn.CONCAT("0",MONTH(B34)),MONTH(B34)),"-",IF(DAY(B34)&lt;10,_xlfn.CONCAT("0",DAY(B34)),DAY(B34)))</f>
+        <v>A6N-13N-62-S217^2018-12-01</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -1956,17 +2048,20 @@
         <v>38026</v>
       </c>
       <c r="E36" s="1">
-        <v>44562</v>
-      </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="2">
+        <v>44570</v>
+      </c>
+      <c r="F36" s="2">
         <v>220000</v>
       </c>
+      <c r="G36" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H36" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I36" s="5">
         <v>33922</v>
+      </c>
+      <c r="I36" t="str">
+        <f>_xlfn.CONCAT(A36,"^",YEAR(B36),"-",IF(MONTH(B36)&lt;10,_xlfn.CONCAT("0",MONTH(B36)),MONTH(B36)),"-",IF(DAY(B36)&lt;10,_xlfn.CONCAT("0",DAY(B36)),DAY(B36)))</f>
+        <v>A6N-13N-62-S219^2004-02-09</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -1987,15 +2082,18 @@
       <c r="E38" s="1">
         <v>44576</v>
       </c>
-      <c r="F38" s="4"/>
-      <c r="G38" s="2">
+      <c r="F38" s="2">
         <v>310000</v>
       </c>
+      <c r="G38" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H38" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I38" s="5">
         <v>29054785</v>
+      </c>
+      <c r="I38" t="str">
+        <f>_xlfn.CONCAT(A38,"^",YEAR(B38),"-",IF(MONTH(B38)&lt;10,_xlfn.CONCAT("0",MONTH(B38)),MONTH(B38)),"-",IF(DAY(B38)&lt;10,_xlfn.CONCAT("0",DAY(B38)),DAY(B38)))</f>
+        <v>A6N-13N-62-S221^2018-06-15</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -2011,14 +2109,18 @@
       <c r="E39" s="1">
         <v>44713</v>
       </c>
-      <c r="G39" s="2">
+      <c r="F39" s="2">
         <v>570000</v>
       </c>
+      <c r="G39" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H39" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I39" s="5">
         <v>19845080</v>
+      </c>
+      <c r="I39" t="str">
+        <f>_xlfn.CONCAT(A39,"^",YEAR(B39),"-",IF(MONTH(B39)&lt;10,_xlfn.CONCAT("0",MONTH(B39)),MONTH(B39)),"-",IF(DAY(B39)&lt;10,_xlfn.CONCAT("0",DAY(B39)),DAY(B39)))</f>
+        <v>A6N-13N-62-S222^2022-06-01</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -2037,15 +2139,18 @@
       <c r="E40" s="1">
         <v>44562</v>
       </c>
-      <c r="F40" s="4"/>
-      <c r="G40" s="2">
+      <c r="F40" s="2">
         <v>830000</v>
       </c>
+      <c r="G40" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H40" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I40" s="5">
         <v>29434066</v>
+      </c>
+      <c r="I40" t="str">
+        <f>_xlfn.CONCAT(A40,"^",YEAR(B40),"-",IF(MONTH(B40)&lt;10,_xlfn.CONCAT("0",MONTH(B40)),MONTH(B40)),"-",IF(DAY(B40)&lt;10,_xlfn.CONCAT("0",DAY(B40)),DAY(B40)))</f>
+        <v>A6N-13N-62-S301^2021-08-01</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -2062,15 +2167,18 @@
       <c r="E41" s="1">
         <v>44531</v>
       </c>
-      <c r="F41" s="4"/>
-      <c r="G41" s="2">
+      <c r="F41" s="2">
         <v>700000</v>
       </c>
+      <c r="G41" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H41" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I41" s="5">
         <v>1086017</v>
+      </c>
+      <c r="I41" t="str">
+        <f>_xlfn.CONCAT(A41,"^",YEAR(B41),"-",IF(MONTH(B41)&lt;10,_xlfn.CONCAT("0",MONTH(B41)),MONTH(B41)),"-",IF(DAY(B41)&lt;10,_xlfn.CONCAT("0",DAY(B41)),DAY(B41)))</f>
+        <v>A6N-13N-62-S302^2021-08-01</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -2086,15 +2194,18 @@
       <c r="E42" s="1">
         <v>44599</v>
       </c>
-      <c r="F42" s="4"/>
-      <c r="G42" s="2">
+      <c r="F42" s="2">
         <v>700000</v>
       </c>
+      <c r="G42" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H42" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I42" s="5">
         <v>1113686599</v>
+      </c>
+      <c r="I42" t="str">
+        <f>_xlfn.CONCAT(A42,"^",YEAR(B42),"-",IF(MONTH(B42)&lt;10,_xlfn.CONCAT("0",MONTH(B42)),MONTH(B42)),"-",IF(DAY(B42)&lt;10,_xlfn.CONCAT("0",DAY(B42)),DAY(B42)))</f>
+        <v>A6N-13N-62-S303^2022-03-01</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -2104,7 +2215,6 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -2120,15 +2230,18 @@
       <c r="E44" s="4">
         <v>44652</v>
       </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="2">
+      <c r="F44" s="2">
         <v>700000</v>
       </c>
+      <c r="G44" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H44" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I44" s="5">
         <v>31197760</v>
+      </c>
+      <c r="I44" t="str">
+        <f>_xlfn.CONCAT(A44,"^",YEAR(B44),"-",IF(MONTH(B44)&lt;10,_xlfn.CONCAT("0",MONTH(B44)),MONTH(B44)),"-",IF(DAY(B44)&lt;10,_xlfn.CONCAT("0",DAY(B44)),DAY(B44)))</f>
+        <v>A6N-13N-62-S304^2022-04-01</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -2142,17 +2255,20 @@
         <v>44228</v>
       </c>
       <c r="E45" s="1">
-        <v>44197</v>
-      </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="2">
+        <v>44562</v>
+      </c>
+      <c r="F45" s="2">
         <v>750000</v>
       </c>
+      <c r="G45" s="5">
+        <v>19128434</v>
+      </c>
       <c r="H45" s="5">
-        <v>19128434</v>
-      </c>
-      <c r="I45" s="5">
         <v>1115073326</v>
+      </c>
+      <c r="I45" t="str">
+        <f>_xlfn.CONCAT(A45,"^",YEAR(B45),"-",IF(MONTH(B45)&lt;10,_xlfn.CONCAT("0",MONTH(B45)),MONTH(B45)),"-",IF(DAY(B45)&lt;10,_xlfn.CONCAT("0",DAY(B45)),DAY(B45)))</f>
+        <v>A6N-13N-62-S305^2021-02-01</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -2168,15 +2284,18 @@
       <c r="E46" s="1">
         <v>44501</v>
       </c>
-      <c r="F46" s="4"/>
-      <c r="G46" s="2">
+      <c r="F46" s="2">
         <v>420000</v>
       </c>
+      <c r="G46" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H46" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I46" s="5">
         <v>16701786</v>
+      </c>
+      <c r="I46" t="str">
+        <f>_xlfn.CONCAT(A46,"^",YEAR(B46),"-",IF(MONTH(B46)&lt;10,_xlfn.CONCAT("0",MONTH(B46)),MONTH(B46)),"-",IF(DAY(B46)&lt;10,_xlfn.CONCAT("0",DAY(B46)),DAY(B46)))</f>
+        <v>A6N-13N-62-S306^2018-06-01</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -2188,8 +2307,33 @@
       <c r="A48" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B48" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C48" s="1">
+        <v>44621</v>
+      </c>
+      <c r="D48" s="1">
+        <v>44712</v>
+      </c>
+      <c r="E48" s="1">
+        <v>44621</v>
+      </c>
+      <c r="F48" s="2">
+        <v>390000</v>
+      </c>
+      <c r="G48" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="H48" s="5">
+        <v>1144074047</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" ref="I48:I56" si="3">_xlfn.CONCAT(A48,"^",YEAR(B48),"-",IF(MONTH(B48)&lt;10,_xlfn.CONCAT("0",MONTH(B48)),MONTH(B48)),"-",IF(DAY(B48)&lt;10,_xlfn.CONCAT("0",DAY(B48)),DAY(B48)))</f>
+        <v>A6N-13N-62-S308^2022-03-01</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -2202,18 +2346,21 @@
       <c r="E49" s="1">
         <v>44743</v>
       </c>
-      <c r="F49" s="4"/>
-      <c r="G49" s="2">
+      <c r="F49" s="2">
         <v>390000</v>
       </c>
+      <c r="G49" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H49" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I49" s="5">
         <v>1114728401</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I49" t="str">
+        <f t="shared" si="3"/>
+        <v>A6N-13N-62-S308^2022-07-01</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -2226,27 +2373,54 @@
       <c r="E50" s="1">
         <v>44621</v>
       </c>
-      <c r="F50" s="4"/>
-      <c r="G50" s="2">
+      <c r="F50" s="2">
         <v>390000</v>
       </c>
+      <c r="G50" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H50" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I50" s="5">
         <v>61437235</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I50" t="str">
+        <f t="shared" si="3"/>
+        <v>A6N-13N-62-S309^2022-03-01</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="4"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B51" s="1">
+        <v>44531</v>
+      </c>
+      <c r="C51" s="1">
+        <v>44522</v>
+      </c>
+      <c r="D51" s="1">
+        <v>44592</v>
+      </c>
+      <c r="E51" s="1">
+        <v>44562</v>
+      </c>
+      <c r="F51" s="2">
+        <v>390000</v>
+      </c>
+      <c r="G51" s="5">
+        <v>6108014</v>
+      </c>
+      <c r="H51" s="5">
+        <v>14838593</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="3"/>
+        <v>A6N-13N-62-S310^2021-12-01</v>
+      </c>
+      <c r="J51" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -2259,17 +2433,21 @@
       <c r="E52" s="1">
         <v>44743</v>
       </c>
-      <c r="G52" s="2">
+      <c r="F52" s="2">
         <v>390000</v>
       </c>
+      <c r="G52" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H52" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I52" s="5">
         <v>29185053</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I52" t="str">
+        <f t="shared" si="3"/>
+        <v>A6N-13N-62-S310^2022-07-01</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -2282,18 +2460,21 @@
       <c r="E53" s="1">
         <v>44562</v>
       </c>
-      <c r="F53" s="4"/>
-      <c r="G53" s="2">
+      <c r="F53" s="2">
         <v>390000</v>
       </c>
+      <c r="G53" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H53" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I53" s="5">
         <v>1130628991</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I53" t="str">
+        <f t="shared" si="3"/>
+        <v>A6N-13N-62-S311^2021-11-01</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -2306,18 +2487,21 @@
       <c r="E54" s="1">
         <v>44562</v>
       </c>
-      <c r="F54" s="4"/>
-      <c r="G54" s="2">
+      <c r="F54" s="2">
         <v>420000</v>
       </c>
+      <c r="G54" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H54" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I54" s="5">
         <v>1130668637</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I54" t="str">
+        <f t="shared" si="3"/>
+        <v>A6N-13N-62-S312^2017-06-01</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>51</v>
       </c>
@@ -2330,18 +2514,21 @@
       <c r="E55" s="1">
         <v>44562</v>
       </c>
-      <c r="F55" s="4"/>
-      <c r="G55" s="2">
+      <c r="F55" s="2">
         <v>430000</v>
       </c>
+      <c r="G55" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H55" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I55" s="5">
         <v>66818737</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I55" t="str">
+        <f t="shared" si="3"/>
+        <v>A6N-13N-62-S314^2019-06-01</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -2357,22 +2544,26 @@
       <c r="E56" s="1">
         <v>44562</v>
       </c>
-      <c r="G56" s="2">
+      <c r="F56" s="2">
         <v>295000</v>
       </c>
+      <c r="G56" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H56" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I56" s="5">
         <v>1114728401</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I56" t="str">
+        <f t="shared" si="3"/>
+        <v>A6N-13N-62-S315^2019-08-01</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -2385,17 +2576,21 @@
       <c r="E58" s="1">
         <v>44715</v>
       </c>
-      <c r="G58" s="2">
+      <c r="F58" s="2">
         <v>390000</v>
       </c>
+      <c r="G58" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H58" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I58" s="5">
         <v>1125230924</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I58" t="str">
+        <f>_xlfn.CONCAT(A58,"^",YEAR(B58),"-",IF(MONTH(B58)&lt;10,_xlfn.CONCAT("0",MONTH(B58)),MONTH(B58)),"-",IF(DAY(B58)&lt;10,_xlfn.CONCAT("0",DAY(B58)),DAY(B58)))</f>
+        <v>A6N-13N-62-S317^2022-06-01</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -2408,17 +2603,21 @@
       <c r="E59" s="1">
         <v>44562</v>
       </c>
-      <c r="G59" s="2">
+      <c r="F59" s="2">
         <v>290000</v>
       </c>
+      <c r="G59" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H59" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I59" s="5">
         <v>80817426</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I59" t="str">
+        <f>_xlfn.CONCAT(A59,"^",YEAR(B59),"-",IF(MONTH(B59)&lt;10,_xlfn.CONCAT("0",MONTH(B59)),MONTH(B59)),"-",IF(DAY(B59)&lt;10,_xlfn.CONCAT("0",DAY(B59)),DAY(B59)))</f>
+        <v>A6N-13N-62-S318^2021-08-01</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>56</v>
       </c>
@@ -2431,22 +2630,26 @@
       <c r="E60" s="1">
         <v>44562</v>
       </c>
-      <c r="G60" s="2">
+      <c r="F60" s="2">
         <v>470000</v>
       </c>
+      <c r="G60" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H60" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I60" s="5">
         <v>79052475</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I60" t="str">
+        <f>_xlfn.CONCAT(A60,"^",YEAR(B60),"-",IF(MONTH(B60)&lt;10,_xlfn.CONCAT("0",MONTH(B60)),MONTH(B60)),"-",IF(DAY(B60)&lt;10,_xlfn.CONCAT("0",DAY(B60)),DAY(B60)))</f>
+        <v>A6N-13N-62-S319^2021-08-01</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -2457,19 +2660,23 @@
         <v>35290</v>
       </c>
       <c r="E62" s="1">
-        <v>44562</v>
-      </c>
-      <c r="G62" s="2">
+        <v>44574</v>
+      </c>
+      <c r="F62" s="2">
         <v>150000</v>
       </c>
+      <c r="G62" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H62" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I62" s="5">
         <v>31233821</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I62" t="str">
+        <f>_xlfn.CONCAT(A62,"^",YEAR(B62),"-",IF(MONTH(B62)&lt;10,_xlfn.CONCAT("0",MONTH(B62)),MONTH(B62)),"-",IF(DAY(B62)&lt;10,_xlfn.CONCAT("0",DAY(B62)),DAY(B62)))</f>
+        <v>A6N-13N-62-S321^1996-08-13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -2482,17 +2689,21 @@
       <c r="E63" s="1">
         <v>44562</v>
       </c>
-      <c r="G63" s="2">
+      <c r="F63" s="2">
         <v>470000</v>
       </c>
+      <c r="G63" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H63" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I63" s="5">
         <v>94041536</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I63" t="str">
+        <f>_xlfn.CONCAT(A63,"^",YEAR(B63),"-",IF(MONTH(B63)&lt;10,_xlfn.CONCAT("0",MONTH(B63)),MONTH(B63)),"-",IF(DAY(B63)&lt;10,_xlfn.CONCAT("0",DAY(B63)),DAY(B63)))</f>
+        <v>A6N-13N-62-S322^2021-01-01</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -2505,18 +2716,21 @@
       <c r="E64" s="1">
         <v>44562</v>
       </c>
-      <c r="F64" s="4"/>
-      <c r="G64" s="2">
+      <c r="F64" s="2">
         <v>700000</v>
       </c>
+      <c r="G64" s="5">
+        <v>6108014</v>
+      </c>
       <c r="H64" s="5">
-        <v>6108014</v>
-      </c>
-      <c r="I64" s="5">
         <v>70903810</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I64" t="str">
+        <f>_xlfn.CONCAT(A64,"^",YEAR(B64),"-",IF(MONTH(B64)&lt;10,_xlfn.CONCAT("0",MONTH(B64)),MONTH(B64)),"-",IF(DAY(B64)&lt;10,_xlfn.CONCAT("0",DAY(B64)),DAY(B64)))</f>
+        <v>A6N-13N-66^2019-04-01</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -2529,20 +2743,22 @@
       <c r="E65" s="1">
         <v>44562</v>
       </c>
-      <c r="F65" s="4"/>
-      <c r="G65" s="2">
+      <c r="F65" s="2">
         <v>1120000</v>
       </c>
+      <c r="G65" s="5">
+        <v>19245383</v>
+      </c>
       <c r="H65" s="5">
-        <v>19245383</v>
-      </c>
-      <c r="I65" s="5">
         <v>70903810</v>
       </c>
-      <c r="K65" s="1"/>
-      <c r="M65" s="1"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I65" t="str">
+        <f>_xlfn.CONCAT(A65,"^",YEAR(B65),"-",IF(MONTH(B65)&lt;10,_xlfn.CONCAT("0",MONTH(B65)),MONTH(B65)),"-",IF(DAY(B65)&lt;10,_xlfn.CONCAT("0",DAY(B65)),DAY(B65)))</f>
+        <v>A6N-13N-68^1999-02-01</v>
+      </c>
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -2553,7 +2769,7 @@
         <v>44470</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -2564,7 +2780,7 @@
         <v>44631</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>64</v>
       </c>
@@ -2575,12 +2791,12 @@
         <v>44228</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>66</v>
       </c>
@@ -2591,7 +2807,7 @@
         <v>42856</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -2602,7 +2818,7 @@
         <v>44136</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>68</v>
       </c>
@@ -2613,7 +2829,7 @@
         <v>41379</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>69</v>
       </c>
@@ -2621,7 +2837,7 @@
         <v>43009</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>70</v>
       </c>
@@ -2632,7 +2848,7 @@
         <v>43556</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>71</v>
       </c>
@@ -2643,7 +2859,7 @@
         <v>41883</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>72</v>
       </c>
@@ -2654,7 +2870,7 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -2662,7 +2878,7 @@
         <v>42415</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>73</v>
       </c>
@@ -2673,7 +2889,7 @@
         <v>43221</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -2684,7 +2900,7 @@
         <v>38200</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>75</v>
       </c>

</xml_diff>